<commit_message>
modified ERS Testing Documentation.xlsx
</commit_message>
<xml_diff>
--- a/ERS Testing Documentation.xlsx
+++ b/ERS Testing Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41fb85a9a0361d73/Desktop/ERS Testing Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="516" documentId="7_{2EB047B2-1CB8-8749-8564-EAA5D79892DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F46C38A3-5CAC-4AA8-AA2C-121C7F7A9165}"/>
+  <xr:revisionPtr revIDLastSave="524" documentId="7_{2EB047B2-1CB8-8749-8564-EAA5D79892DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90F514E0-6ED2-4114-866C-FB2E00187CD0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="135">
   <si>
     <t>LOGIN</t>
   </si>
@@ -106,9 +106,6 @@
     <t xml:space="preserve">Check login page display </t>
   </si>
   <si>
-    <t xml:space="preserve">Error message about login with vaild credentials </t>
-  </si>
-  <si>
     <t xml:space="preserve">User Story </t>
   </si>
   <si>
@@ -225,14 +222,6 @@
   <si>
     <t>Username = &lt;blank&gt; 
 Password  = &lt;blank&gt;</t>
-  </si>
-  <si>
-    <t>Username = &lt;incorrect&gt; 
-Password  = Passw@rd</t>
-  </si>
-  <si>
-    <t>Username = abc1234
-Password = &lt;incorrect&gt;</t>
   </si>
   <si>
     <t>Empolyee Reimbursement</t>
@@ -520,6 +509,22 @@
   <si>
     <t>Display error message as:
 "Username and Password does not match. Please try again with correct credentials !!!"</t>
+  </si>
+  <si>
+    <t>Username = bipul51
+Password  = password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display error message as:
+"Username and Password does not match. Please try again with correct credentials !!!" </t>
+  </si>
+  <si>
+    <t>Username and Password does not match._x000D_
+ Please try again with correct credentials !!!</t>
+  </si>
+  <si>
+    <t>Username = abc1234
+Password = testing123</t>
   </si>
 </sst>
 </file>
@@ -917,74 +922,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1008,7 +1013,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1018,58 +1023,58 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
         <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
         <v>51</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1085,7 +1090,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,19 +1119,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
@@ -1143,16 +1148,16 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1166,7 +1171,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
@@ -1175,7 +1180,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1189,16 +1194,16 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1212,12 +1217,17 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="6"/>
+        <v>131</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1230,10 +1240,16 @@
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
+        <v>134</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1266,7 +1282,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1278,22 +1294,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>2</v>
@@ -1301,155 +1317,155 @@
     </row>
     <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
       <c r="E4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
         <v>75</v>
-      </c>
-      <c r="B6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
         <v>87</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
         <v>81</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" t="s">
-        <v>94</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
         <v>95</v>
       </c>
-      <c r="B10" t="s">
-        <v>98</v>
-      </c>
       <c r="C10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
         <v>97</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1481,7 +1497,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1495,22 +1511,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>2</v>
@@ -1518,87 +1534,87 @@
     </row>
     <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" t="s">
         <v>113</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>114</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
         <v>118</v>
-      </c>
-      <c r="B6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" t="s">
         <v>123</v>
-      </c>
-      <c r="B7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify ERS Testing Documentation.xlsx and add Test Report.xlsx
</commit_message>
<xml_diff>
--- a/ERS Testing Documentation.xlsx
+++ b/ERS Testing Documentation.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="621" documentId="7_{2EB047B2-1CB8-8749-8564-EAA5D79892DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96137C47-2E87-4F90-A03B-BFD29B3C9A1F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2124" yWindow="2448" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accpetance Criteria" sheetId="2" r:id="rId1"/>
@@ -1110,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A785BB-A14E-4D41-838B-24B4BC718318}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1287,7 +1287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFB9951-19D4-4B96-B2E4-D41F363B21EA}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1546,7 +1546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C458FD20-DBAF-42C4-9DB4-71E59F978B4F}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modify ERS Testing Documentation.xlsx and Test Report.xlsx
</commit_message>
<xml_diff>
--- a/ERS Testing Documentation.xlsx
+++ b/ERS Testing Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41fb85a9a0361d73/Desktop/ERS Testing Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="621" documentId="7_{2EB047B2-1CB8-8749-8564-EAA5D79892DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96137C47-2E87-4F90-A03B-BFD29B3C9A1F}"/>
+  <xr:revisionPtr revIDLastSave="622" documentId="7_{2EB047B2-1CB8-8749-8564-EAA5D79892DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69017133-4A8A-4DCA-9FC0-4D0A36F3E951}"/>
   <bookViews>
-    <workbookView xWindow="2124" yWindow="2448" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accpetance Criteria" sheetId="2" r:id="rId1"/>
@@ -929,6 +929,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5593F422-5F63-5447-BEEA-526AAF00421E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>